<commit_message>
docs: several text and image fixes
fixed some sentences and all the images

Signed-off-by: Carlos Souza <carlos.souza@analog.com>
</commit_message>
<xml_diff>
--- a/docs/library/xilinx/util_adxcvr/xcvr_mapping_example.xlsx
+++ b/docs/library/xilinx/util_adxcvr/xcvr_mapping_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Xilinx_2023.1-Ubuntu-22.04\home\caosjr\HDL-fork\hdl\docs\library\xilinx\util_adxcvr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Xilinx_2023.1-Ubuntu-22.04\home\caosjr\HDL-analog\hdl\docs\library\xilinx\util_adxcvr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DE8614-53B9-43A0-9AF4-D1025AFA9592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC09C4F1-CBD8-4FDD-9228-B4BE41F1931A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{78997C56-A9F3-4AB3-B876-092FAD5E3946}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{78997C56-A9F3-4AB3-B876-092FAD5E3946}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -614,17 +614,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="1"/>
       </left>
       <right style="thin">
         <color theme="2"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="medium">
         <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,11 +648,9 @@
       <right style="thin">
         <color theme="2"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="medium">
         <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,54 +661,7 @@
       <right style="medium">
         <color theme="1"/>
       </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2"/>
-      </left>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color theme="1"/>
       </bottom>
@@ -707,79 +671,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04926D4C-C525-4399-BFD2-FA8EDE69F454}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,174 +1059,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="25" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="25" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="25" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="25" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1289,7 +1241,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,190 +1257,190 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="41" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="3"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="35" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
@@ -1570,7 +1522,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
+      <selection activeCellId="2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,196 +1537,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="41" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="3"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="29" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="32"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1789,10 +1741,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC25F7EF-F632-4AA7-BA07-5D3FB1987E6B}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,186 +1759,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="21"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="3"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="35" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="32"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>